<commit_message>
finalized paper and gaant chart
</commit_message>
<xml_diff>
--- a/Project Gannt Chart.xlsx
+++ b/Project Gannt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E01289B-6758-CC4A-B664-4D3B110A70EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41F104F-AF8A-6449-ADB9-542C1253DBE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Create Procedures, Views, and Indexes</t>
+  </si>
+  <si>
+    <t>Implement Poster</t>
   </si>
 </sst>
 </file>
@@ -704,7 +707,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -903,15 +906,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="12" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -923,36 +959,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="12" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1520,11 +1526,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL33"/>
+  <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24:D24"/>
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1564,15 +1570,15 @@
       <c r="B2" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="79">
+      <c r="D2" s="86"/>
+      <c r="E2" s="81">
         <f>DATE(2020, 11, 28)</f>
         <v>44163</v>
       </c>
-      <c r="F2" s="80"/>
+      <c r="F2" s="82"/>
       <c r="I2" s="53" t="s">
         <v>16</v>
       </c>
@@ -1584,107 +1590,107 @@
       <c r="B3" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="79">
+      <c r="D3" s="88"/>
+      <c r="E3" s="81">
         <f>DATE(2020, 10, 20)</f>
         <v>44124</v>
       </c>
-      <c r="F3" s="80"/>
+      <c r="F3" s="82"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="82">
+      <c r="I4" s="78">
         <f>I5</f>
         <v>44123</v>
       </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="82">
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="78">
         <f>P5</f>
         <v>44130</v>
       </c>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="82">
+      <c r="Q4" s="79"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="79"/>
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="78">
         <f>W5</f>
         <v>44137</v>
       </c>
-      <c r="X4" s="83"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="83"/>
-      <c r="AB4" s="83"/>
-      <c r="AC4" s="84"/>
-      <c r="AD4" s="82">
+      <c r="X4" s="79"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="79"/>
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="78">
         <f>AD5</f>
         <v>44144</v>
       </c>
-      <c r="AE4" s="83"/>
-      <c r="AF4" s="83"/>
-      <c r="AG4" s="83"/>
-      <c r="AH4" s="83"/>
-      <c r="AI4" s="83"/>
-      <c r="AJ4" s="84"/>
-      <c r="AK4" s="82">
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="79"/>
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="80"/>
+      <c r="AK4" s="78">
         <f>AK5</f>
         <v>44151</v>
       </c>
-      <c r="AL4" s="83"/>
-      <c r="AM4" s="83"/>
-      <c r="AN4" s="83"/>
-      <c r="AO4" s="83"/>
-      <c r="AP4" s="83"/>
-      <c r="AQ4" s="84"/>
-      <c r="AR4" s="82">
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="79"/>
+      <c r="AN4" s="79"/>
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="80"/>
+      <c r="AR4" s="78">
         <f>AR5</f>
         <v>44158</v>
       </c>
-      <c r="AS4" s="83"/>
-      <c r="AT4" s="83"/>
-      <c r="AU4" s="83"/>
-      <c r="AV4" s="83"/>
-      <c r="AW4" s="83"/>
-      <c r="AX4" s="84"/>
-      <c r="AY4" s="82">
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="78">
         <f>AY5</f>
         <v>44165</v>
       </c>
-      <c r="AZ4" s="83"/>
-      <c r="BA4" s="83"/>
-      <c r="BB4" s="83"/>
-      <c r="BC4" s="83"/>
-      <c r="BD4" s="83"/>
-      <c r="BE4" s="84"/>
-      <c r="BF4" s="82">
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="79"/>
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="78">
         <f>BF5</f>
         <v>44172</v>
       </c>
-      <c r="BG4" s="83"/>
-      <c r="BH4" s="83"/>
-      <c r="BI4" s="83"/>
-      <c r="BJ4" s="83"/>
-      <c r="BK4" s="83"/>
-      <c r="BL4" s="84"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="79"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="80"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
@@ -1928,10 +1934,10 @@
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="89"/>
       <c r="E6" s="8" t="s">
         <v>4</v>
       </c>
@@ -2247,7 +2253,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="str">
-        <f t="shared" ref="H8:H30" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H32" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="36"/>
@@ -2314,10 +2320,10 @@
       <c r="B9" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="81"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="58">
         <f>Project_Start</f>
         <v>44124</v>
@@ -2395,10 +2401,10 @@
       <c r="B10" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="72"/>
+      <c r="D10" s="84"/>
       <c r="E10" s="58">
         <f>F9</f>
         <v>44128</v>
@@ -2474,10 +2480,10 @@
       <c r="B11" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="72"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="58">
         <f>F10</f>
         <v>44130</v>
@@ -2553,10 +2559,10 @@
       <c r="B12" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="72"/>
+      <c r="D12" s="84"/>
       <c r="E12" s="58">
         <f>F11-1</f>
         <v>44135</v>
@@ -2632,10 +2638,10 @@
       <c r="B13" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="72"/>
+      <c r="D13" s="84"/>
       <c r="E13" s="58">
         <f>F12 - 1</f>
         <v>44137</v>
@@ -2713,8 +2719,8 @@
       <c r="B14" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
       <c r="E14" s="22"/>
       <c r="F14" s="23"/>
       <c r="G14" s="16"/>
@@ -2784,10 +2790,10 @@
       <c r="B15" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="74"/>
+      <c r="D15" s="76"/>
       <c r="E15" s="59">
         <f>F13+1</f>
         <v>44139</v>
@@ -2863,10 +2869,10 @@
       <c r="B16" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="74"/>
+      <c r="D16" s="76"/>
       <c r="E16" s="59">
         <f>E15</f>
         <v>44139</v>
@@ -2942,10 +2948,10 @@
       <c r="B17" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="74"/>
+      <c r="D17" s="76"/>
       <c r="E17" s="59">
         <f>F16</f>
         <v>44142</v>
@@ -3021,10 +3027,10 @@
       <c r="B18" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="74"/>
+      <c r="D18" s="76"/>
       <c r="E18" s="59">
         <f>F17 + 1</f>
         <v>44149</v>
@@ -3102,8 +3108,8 @@
       <c r="B19" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
       <c r="G19" s="16"/>
@@ -3173,10 +3179,10 @@
       <c r="B20" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="86"/>
+      <c r="D20" s="74"/>
       <c r="E20" s="60">
         <f>F15</f>
         <v>44153</v>
@@ -3252,10 +3258,10 @@
       <c r="B21" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="86"/>
+      <c r="D21" s="74"/>
       <c r="E21" s="60">
         <f>F18 + 1</f>
         <v>44157</v>
@@ -3331,10 +3337,10 @@
       <c r="B22" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="86"/>
+      <c r="D22" s="74"/>
       <c r="E22" s="60">
         <f>F21 + 1</f>
         <v>44160</v>
@@ -3410,10 +3416,10 @@
       <c r="B23" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="86"/>
+      <c r="D23" s="74"/>
       <c r="E23" s="60">
         <f>F22</f>
         <v>44161</v>
@@ -3486,10 +3492,10 @@
       <c r="B24" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="86"/>
+      <c r="D24" s="74"/>
       <c r="E24" s="60">
         <f>F23</f>
         <v>44163</v>
@@ -3567,8 +3573,8 @@
       <c r="B25" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
       <c r="E25" s="28"/>
       <c r="F25" s="29"/>
       <c r="G25" s="16"/>
@@ -3638,10 +3644,10 @@
       <c r="B26" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="88" t="s">
+      <c r="C26" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="88"/>
+      <c r="D26" s="73"/>
       <c r="E26" s="61">
         <f>E24</f>
         <v>44163</v>
@@ -3717,22 +3723,22 @@
       <c r="B27" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="88"/>
+      <c r="D27" s="73"/>
       <c r="E27" s="61">
         <f>F26</f>
         <v>44164</v>
       </c>
       <c r="F27" s="61">
-        <f>E27+2</f>
-        <v>44166</v>
+        <f>E27+1</f>
+        <v>44165</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I27" s="36"/>
       <c r="J27" s="36"/>
@@ -3796,10 +3802,10 @@
       <c r="B28" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="88" t="s">
+      <c r="C28" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="88"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="61">
         <f>F20</f>
         <v>44164</v>
@@ -3809,10 +3815,7 @@
         <v>44166</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28" s="16">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
+      <c r="H28" s="16"/>
       <c r="I28" s="36"/>
       <c r="J28" s="36"/>
       <c r="K28" s="36"/>
@@ -3871,19 +3874,24 @@
       <c r="BL28" s="36"/>
     </row>
     <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="72"/>
+      <c r="E29" s="61">
+        <f>E28+1</f>
+        <v>44165</v>
+      </c>
+      <c r="F29" s="61">
+        <f>E29+1</f>
+        <v>44166</v>
+      </c>
       <c r="G29" s="16"/>
-      <c r="H29" s="16" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H29" s="16"/>
       <c r="I29" s="36"/>
       <c r="J29" s="36"/>
       <c r="K29" s="36"/>
@@ -3942,103 +3950,253 @@
       <c r="BL29" s="36"/>
     </row>
     <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35" t="str">
+      <c r="A30" s="50"/>
+      <c r="B30" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="73"/>
+      <c r="E30" s="61">
+        <f>F28</f>
+        <v>44166</v>
+      </c>
+      <c r="F30" s="61">
+        <f>E30</f>
+        <v>44166</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="36"/>
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
+      <c r="AA30" s="36"/>
+      <c r="AB30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="36"/>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="36"/>
+      <c r="AH30" s="36"/>
+      <c r="AI30" s="36"/>
+      <c r="AJ30" s="36"/>
+      <c r="AK30" s="36"/>
+      <c r="AL30" s="36"/>
+      <c r="AM30" s="36"/>
+      <c r="AN30" s="36"/>
+      <c r="AO30" s="36"/>
+      <c r="AP30" s="36"/>
+      <c r="AQ30" s="36"/>
+      <c r="AR30" s="36"/>
+      <c r="AS30" s="36"/>
+      <c r="AT30" s="36"/>
+      <c r="AU30" s="36"/>
+      <c r="AV30" s="36"/>
+      <c r="AW30" s="36"/>
+      <c r="AX30" s="36"/>
+      <c r="AY30" s="36"/>
+      <c r="AZ30" s="36"/>
+      <c r="BA30" s="36"/>
+      <c r="BB30" s="36"/>
+      <c r="BC30" s="36"/>
+      <c r="BD30" s="36"/>
+      <c r="BE30" s="36"/>
+      <c r="BF30" s="36"/>
+      <c r="BG30" s="36"/>
+      <c r="BH30" s="36"/>
+      <c r="BI30" s="36"/>
+      <c r="BJ30" s="36"/>
+      <c r="BK30" s="36"/>
+      <c r="BL30" s="36"/>
+    </row>
+    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="69"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="38"/>
-      <c r="U30" s="38"/>
-      <c r="V30" s="38"/>
-      <c r="W30" s="38"/>
-      <c r="X30" s="38"/>
-      <c r="Y30" s="38"/>
-      <c r="Z30" s="38"/>
-      <c r="AA30" s="38"/>
-      <c r="AB30" s="38"/>
-      <c r="AC30" s="38"/>
-      <c r="AD30" s="38"/>
-      <c r="AE30" s="38"/>
-      <c r="AF30" s="38"/>
-      <c r="AG30" s="38"/>
-      <c r="AH30" s="38"/>
-      <c r="AI30" s="38"/>
-      <c r="AJ30" s="38"/>
-      <c r="AK30" s="38"/>
-      <c r="AL30" s="38"/>
-      <c r="AM30" s="38"/>
-      <c r="AN30" s="38"/>
-      <c r="AO30" s="38"/>
-      <c r="AP30" s="38"/>
-      <c r="AQ30" s="38"/>
-      <c r="AR30" s="38"/>
-      <c r="AS30" s="38"/>
-      <c r="AT30" s="38"/>
-      <c r="AU30" s="38"/>
-      <c r="AV30" s="38"/>
-      <c r="AW30" s="38"/>
-      <c r="AX30" s="38"/>
-      <c r="AY30" s="38"/>
-      <c r="AZ30" s="38"/>
-      <c r="BA30" s="38"/>
-      <c r="BB30" s="38"/>
-      <c r="BC30" s="38"/>
-      <c r="BD30" s="38"/>
-      <c r="BE30" s="38"/>
-      <c r="BF30" s="38"/>
-      <c r="BG30" s="38"/>
-      <c r="BH30" s="38"/>
-      <c r="BI30" s="38"/>
-      <c r="BJ30" s="38"/>
-      <c r="BK30" s="38"/>
-      <c r="BL30" s="38"/>
-    </row>
-    <row r="31" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="13"/>
-      <c r="F32" s="52"/>
-    </row>
-    <row r="33" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="14"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="36"/>
+      <c r="AF31" s="36"/>
+      <c r="AG31" s="36"/>
+      <c r="AH31" s="36"/>
+      <c r="AI31" s="36"/>
+      <c r="AJ31" s="36"/>
+      <c r="AK31" s="36"/>
+      <c r="AL31" s="36"/>
+      <c r="AM31" s="36"/>
+      <c r="AN31" s="36"/>
+      <c r="AO31" s="36"/>
+      <c r="AP31" s="36"/>
+      <c r="AQ31" s="36"/>
+      <c r="AR31" s="36"/>
+      <c r="AS31" s="36"/>
+      <c r="AT31" s="36"/>
+      <c r="AU31" s="36"/>
+      <c r="AV31" s="36"/>
+      <c r="AW31" s="36"/>
+      <c r="AX31" s="36"/>
+      <c r="AY31" s="36"/>
+      <c r="AZ31" s="36"/>
+      <c r="BA31" s="36"/>
+      <c r="BB31" s="36"/>
+      <c r="BC31" s="36"/>
+      <c r="BD31" s="36"/>
+      <c r="BE31" s="36"/>
+      <c r="BF31" s="36"/>
+      <c r="BG31" s="36"/>
+      <c r="BH31" s="36"/>
+      <c r="BI31" s="36"/>
+      <c r="BJ31" s="36"/>
+      <c r="BK31" s="36"/>
+      <c r="BL31" s="36"/>
+    </row>
+    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="38"/>
+      <c r="T32" s="38"/>
+      <c r="U32" s="38"/>
+      <c r="V32" s="38"/>
+      <c r="W32" s="38"/>
+      <c r="X32" s="38"/>
+      <c r="Y32" s="38"/>
+      <c r="Z32" s="38"/>
+      <c r="AA32" s="38"/>
+      <c r="AB32" s="38"/>
+      <c r="AC32" s="38"/>
+      <c r="AD32" s="38"/>
+      <c r="AE32" s="38"/>
+      <c r="AF32" s="38"/>
+      <c r="AG32" s="38"/>
+      <c r="AH32" s="38"/>
+      <c r="AI32" s="38"/>
+      <c r="AJ32" s="38"/>
+      <c r="AK32" s="38"/>
+      <c r="AL32" s="38"/>
+      <c r="AM32" s="38"/>
+      <c r="AN32" s="38"/>
+      <c r="AO32" s="38"/>
+      <c r="AP32" s="38"/>
+      <c r="AQ32" s="38"/>
+      <c r="AR32" s="38"/>
+      <c r="AS32" s="38"/>
+      <c r="AT32" s="38"/>
+      <c r="AU32" s="38"/>
+      <c r="AV32" s="38"/>
+      <c r="AW32" s="38"/>
+      <c r="AX32" s="38"/>
+      <c r="AY32" s="38"/>
+      <c r="AZ32" s="38"/>
+      <c r="BA32" s="38"/>
+      <c r="BB32" s="38"/>
+      <c r="BC32" s="38"/>
+      <c r="BD32" s="38"/>
+      <c r="BE32" s="38"/>
+      <c r="BF32" s="38"/>
+      <c r="BG32" s="38"/>
+      <c r="BH32" s="38"/>
+      <c r="BI32" s="38"/>
+      <c r="BJ32" s="38"/>
+      <c r="BK32" s="38"/>
+      <c r="BL32" s="38"/>
+    </row>
+    <row r="33" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="13"/>
+      <c r="F34" s="52"/>
+    </row>
+    <row r="35" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
+  <mergeCells count="35">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
@@ -4047,21 +4205,22 @@
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D8 D29:D30">
+  <conditionalFormatting sqref="D7:D8 D31:D32">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4075,12 +4234,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL30">
+  <conditionalFormatting sqref="I5:BL32">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL30">
+  <conditionalFormatting sqref="I7:BL32">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4119,7 +4278,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D8 D29:D30</xm:sqref>
+          <xm:sqref>D7:D8 D31:D32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>